<commit_message>
Alterações do Caso de Teste Manter Sprint
Alterações do Caso de Teste Manter Sprint
</commit_message>
<xml_diff>
--- a/trunk/doc/testes/CT - Manter Sprint.xlsx
+++ b/trunk/doc/testes/CT - Manter Sprint.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="600" windowWidth="19815" windowHeight="7365"/>
+    <workbookView xWindow="390" yWindow="600" windowWidth="19815" windowHeight="7365" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Capa" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Scrumming</t>
   </si>
@@ -91,12 +91,43 @@
     <t>Sprint deverá ser desativada com sucesso.
 A mensagem de confirmação "Operação realizada com sucesso" deverá ser exibida.</t>
   </si>
+  <si>
+    <t>Efetuar sem sucesso o cadastro de um Sprint. Usuário sem permissão a funcionalidade.</t>
+  </si>
+  <si>
+    <t>1- Tentar executar o passo #1 com usuário sem acesso a funcionalidade.</t>
+  </si>
+  <si>
+    <t>O sistema não deverá exibir a opção para cadastro de Sprint.</t>
+  </si>
+  <si>
+    <t>Efetuar sem sucesso o cadastro de um Sprint. Dados inválidos.
+Passo #1 deverá ter sido executado com sucesso.</t>
+  </si>
+  <si>
+    <t>1- Preencher os campos de cadastro da Sprint com dados inválidos.
+2- Acionar o Salvar.</t>
+  </si>
+  <si>
+    <t>O sistema não deverá salvar a Sprint e deverá exibir uma mensagem de erro informando os campos com preenchimento inválido.</t>
+  </si>
+  <si>
+    <t>Efetuar sem sucesso o cadastro de um Sprint. Campos obrigatórios não preenchidos.
+Passo #1 deverá ter sido executado com sucesso.</t>
+  </si>
+  <si>
+    <t>1- Não preencher os campos obrigatórios do cadastro da Sprint.
+2- Acionar o Salvar.</t>
+  </si>
+  <si>
+    <t>O sistema não deverá salvar a Sprint e deverá exibir uma mensagem de erro informando que os campos estão em branco.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="8">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -160,7 +191,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -182,12 +213,20 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -266,6 +305,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -300,6 +340,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Escritório">
@@ -475,28 +516,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.5703125" customWidth="1"/>
     <col min="2" max="2" width="21.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2" ht="44.25">
+    <row r="2" spans="2:2" ht="44.25" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:2" ht="18">
+    <row r="5" spans="2:2" ht="18" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="2:2" ht="15.75" customHeight="1">
+    <row r="7" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="3"/>
     </row>
   </sheetData>
@@ -505,18 +546,18 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19.42578125" customWidth="1"/>
     <col min="2" max="2" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -524,7 +565,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1">
+    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
         <v>9</v>
       </c>
@@ -532,11 +573,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1">
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
     </row>
-    <row r="4" spans="1:2" ht="15.75" customHeight="1">
+    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="8"/>
       <c r="B4" s="8"/>
     </row>
@@ -546,12 +587,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="3" customWidth="1"/>
     <col min="2" max="2" width="64.28515625" customWidth="1"/>
@@ -559,7 +602,7 @@
     <col min="4" max="4" width="62.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" customHeight="1">
+    <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>4</v>
       </c>
@@ -573,7 +616,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="89.25">
+    <row r="2" spans="1:4" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -587,7 +630,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="51">
+    <row r="3" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -601,7 +644,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="38.25">
+    <row r="4" spans="1:4" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -615,31 +658,49 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="12.75">
+    <row r="5" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
         <v>4</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-    </row>
-    <row r="6" spans="1:4" ht="12.75">
+      <c r="B5" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
         <v>5</v>
       </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-    </row>
-    <row r="7" spans="1:4" ht="12.75">
+      <c r="B6" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
         <v>6</v>
       </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-    </row>
-    <row r="8" spans="1:4" ht="12.75">
+      <c r="B7" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -647,7 +708,7 @@
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
     </row>
-    <row r="9" spans="1:4" ht="12.75">
+    <row r="9" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -655,7 +716,7 @@
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
     </row>
-    <row r="10" spans="1:4" ht="12.75">
+    <row r="10" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -663,7 +724,7 @@
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
     </row>
-    <row r="11" spans="1:4" ht="12.75">
+    <row r="11" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="4">
         <v>10</v>
       </c>
@@ -671,7 +732,7 @@
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
     </row>
-    <row r="12" spans="1:4" ht="12.75">
+    <row r="12" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="4">
         <v>11</v>
       </c>
@@ -679,7 +740,7 @@
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
     </row>
-    <row r="13" spans="1:4" ht="12.75">
+    <row r="13" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="4">
         <v>12</v>
       </c>
@@ -687,117 +748,117 @@
       <c r="C13" s="9"/>
       <c r="D13" s="9"/>
     </row>
-    <row r="14" spans="1:4" ht="15.75" customHeight="1">
+    <row r="14" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4"/>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
     </row>
-    <row r="15" spans="1:4" ht="15.75" customHeight="1">
+    <row r="15" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4"/>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
     </row>
-    <row r="16" spans="1:4" ht="15.75" customHeight="1">
+    <row r="16" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
     </row>
-    <row r="17" spans="1:4" ht="15.75" customHeight="1">
+    <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4"/>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
     </row>
-    <row r="18" spans="1:4" ht="15.75" customHeight="1">
+    <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4"/>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
     </row>
-    <row r="19" spans="1:4" ht="15.75" customHeight="1">
+    <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="4"/>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
     </row>
-    <row r="20" spans="1:4" ht="15.75" customHeight="1">
+    <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="4"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
     </row>
-    <row r="21" spans="1:4" ht="15.75" customHeight="1">
+    <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="4"/>
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
     </row>
-    <row r="22" spans="1:4" ht="15.75" customHeight="1">
+    <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="4"/>
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
     </row>
-    <row r="23" spans="1:4" ht="15.75" customHeight="1">
+    <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="4"/>
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
       <c r="D23" s="7"/>
     </row>
-    <row r="24" spans="1:4" ht="15.75" customHeight="1">
+    <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
       <c r="D24" s="7"/>
     </row>
-    <row r="25" spans="1:4" ht="15.75" customHeight="1">
+    <row r="25" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="7"/>
       <c r="C25" s="7"/>
       <c r="D25" s="7"/>
     </row>
-    <row r="26" spans="1:4" ht="15.75" customHeight="1">
+    <row r="26" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="7"/>
       <c r="C26" s="7"/>
       <c r="D26" s="7"/>
     </row>
-    <row r="27" spans="1:4" ht="15.75" customHeight="1">
+    <row r="27" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="7"/>
       <c r="C27" s="7"/>
       <c r="D27" s="7"/>
     </row>
-    <row r="28" spans="1:4" ht="15.75" customHeight="1">
+    <row r="28" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="7"/>
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
     </row>
-    <row r="29" spans="1:4" ht="15.75" customHeight="1">
+    <row r="29" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="7"/>
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
     </row>
-    <row r="30" spans="1:4" ht="15.75" customHeight="1">
+    <row r="30" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="7"/>
       <c r="C30" s="7"/>
       <c r="D30" s="7"/>
     </row>
-    <row r="31" spans="1:4" ht="15.75" customHeight="1">
+    <row r="31" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="7"/>
       <c r="C31" s="7"/>
       <c r="D31" s="7"/>
     </row>
-    <row r="32" spans="1:4" ht="15.75" customHeight="1">
+    <row r="32" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B32" s="7"/>
       <c r="C32" s="7"/>
       <c r="D32" s="7"/>
     </row>
-    <row r="33" spans="2:4" ht="15.75" customHeight="1">
+    <row r="33" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="7"/>
       <c r="C33" s="7"/>
       <c r="D33" s="7"/>
     </row>
-    <row r="34" spans="2:4" ht="15.75" customHeight="1">
+    <row r="34" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B34" s="7"/>
       <c r="C34" s="7"/>
       <c r="D34" s="7"/>

</xml_diff>